<commit_message>
finished testing with gui time to make webapp
</commit_message>
<xml_diff>
--- a/Candidate Register pep4_5.xlsx
+++ b/Candidate Register pep4_5.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>EXAMID</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>TEL_NUM</t>
+  </si>
+  <si>
+    <t>PAPER04</t>
   </si>
 </sst>
 </file>
@@ -149,9 +152,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,11 +462,12 @@
     <col min="18" max="19" width="1.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" style="1" customWidth="1"/>
     <col min="21" max="22" width="25.7109375" style="1" customWidth="1"/>
-    <col min="23" max="26" width="20.7109375" style="1" customWidth="1"/>
-    <col min="27" max="29" width="50.7109375" style="1" customWidth="1"/>
+    <col min="23" max="27" width="20.7109375" style="1" customWidth="1"/>
+    <col min="28" max="30" width="50.7109375" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,15 +544,18 @@
         <v>22</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>